<commit_message>
updated data files, change model config settings, scaling works
</commit_message>
<xml_diff>
--- a/mppsteel/data/import_data/Scope 1 Emissions Factors.xlsx
+++ b/mppsteel/data/import_data/Scope 1 Emissions Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafalMalinowski\OneDrive - SYSTEMIQ Ltd\Desktop\New inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{FAC0754F-6012-4F70-B556-ECA6018A2F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A5D7DA8-66DF-4285-BF7F-4F1333938054}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD661D5-67F6-48DF-8503-DAC957C08B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4510" yWindow="-16110" windowWidth="25820" windowHeight="15620" xr2:uid="{E80D5846-EB8E-4ACA-AD71-6C7A73B480F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{E80D5846-EB8E-4ACA-AD71-6C7A73B480F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,18 +469,18 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.29296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.1171875" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -514,10 +514,10 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -534,7 +534,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -551,7 +551,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -568,7 +568,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -582,10 +582,10 @@
         <v>8</v>
       </c>
       <c r="E6">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+        <v>191.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2020</v>
       </c>
@@ -602,7 +602,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2020</v>
       </c>
@@ -620,7 +620,7 @@
         <v>78.833333333333343</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -637,7 +637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -654,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2020</v>
       </c>
@@ -671,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -688,60 +688,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
     </row>
   </sheetData>
@@ -750,8 +750,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cc653c178d9ffcb24786b6a9d53371f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3af53c5407280ad7b07c166bc7f6511a" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="378483659bd2bdffed7f8c2e23044a13">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d05f4d662bc807bc82519ff4863d1bb" ns2:_="" ns3:_="">
     <xsd:import namespace="b44fa922-a688-4301-8945-67f7597c9c55"/>
     <xsd:import namespace="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
     <xsd:element name="properties">
@@ -772,6 +781,8 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -835,6 +846,13 @@
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="6fd27762-0251-4a48-b483-e1f79c0a6546" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" elementFormDefault="qualified">
@@ -865,6 +883,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="20" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{2f1cb957-661d-4683-93b6-7eb55a432899}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="f6f44a7d-d6f5-4042-8792-19cb5f90fb06">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -966,31 +995,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <TaxCatchAll xmlns="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b44fa922-a688-4301-8945-67f7597c9c55">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27671131-2B62-4A55-BF4D-0F2C0B6AD7CA}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99619CCA-E26B-4688-AD26-F7EFBE9A5C0F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE120E28-727F-45E2-B7B3-04E2DDA6E832}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>